<commit_message>
6.7 Add Investigate Panel
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/10_Ran.xlsx
+++ b/Assets/StreamingAssets/10_Ran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DCF73C-3942-4944-BA0B-50931D890B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7E7368-EC27-A24F-9F2F-455C8ED9F6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="84">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,211 +133,243 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lee-Regular</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lee-Thinking2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ran医生，请问有结果了吗？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ran医生点了点头，但是一向冷静的她，眼神中透露出动摇和疑惑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>庄主的死亡原因是什么？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ran</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>全身多处受到利刃伤害</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>胸腹部的贯穿伤是致命伤，其他都是皮外伤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>死因是伤重不治，流血过多，不是当场死亡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>庄主的死亡时间是？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>众所周知气温是会改变尸体条件的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今晚有风有雨，阴湿寒冷，又因为死者常年练武，肌肉结实</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>因此尸体僵硬的出现时间比正常情况下要慢</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>刚才庄主尸体的下颌部分已经开始有僵硬现象，目前还为扩撒到全身</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>尸斑已经初步显现，我推测死亡时间是戊初初刻刀戊正初刻之间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>这时间正好是从原定晚宴开始的时间，到真正开始的时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>这么算来，凶手和庄主在庄外厮杀的时间大致可以确定了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>凶手可能是晚宴开始之前作案，之后便装作若无其事回到庄内出席晚宴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>也有可能是在晚宴期间暂时离席，杀害庄主之后再回到宴会厅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据何管家的证词，庄主酉正二刻依然在世</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>那么凶手袭击他的时间范围是：酉正三刻到戌初，大概三刻左右</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以说一下尸体身上衣物的状态吗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全身衣物湿透，但是因为雨水冲刷，衣物上并没有太多血迹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>鞋底和身前的衣服上沾满了泥土和碎草，特别是膝盖和手肘的位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>双手手账和指甲里都有大量泥土</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请问何管家，你最后一次见到庄主时他的衣服是这样的状态吗？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>He</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>当然不是，庄主是朝廷官员，今天是他的寿诞，他必定打扮的仪表堂堂</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>如此说来，庄主身上的泥土可能是因为和凶手打斗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以详细说一下尸体的双手情况吗？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手掌有习武之人的手茧，此外双手有粗绳的勒痕</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从虎口贯穿整个手掌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Yao</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>先生，莫非庄主生前被人捆绑囚禁过？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>似乎不是，如果是捆绑囚禁，手部的勒痕一般会出现在手腕或者手肘位置，而且勒痕应该是环绕一圈的样子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>庄主的勒痕只在手掌内侧，手背却完全没有</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>这道痕迹清晰明显，是死前不久造成的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今天的初步检查到此结束，明天上午我会做更详细的检查</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ran医生辛苦了，请问可以再多问你几个问题吗？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>她没有说话，应该算是默许了吧</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请问你最后一次见到庄主是什么时候？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是昨天为他看病的时候</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我本身应该在昨天下山的，因为要给Lee换药才留到了今天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今天傍晚，快要下雨的时候，你没有见到庄主吗？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>梅夫人突然卧病，庄主说想邀请你去医治</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ran摇了摇头</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以说一下晚宴前后的行动吗？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>晚宴之后从未离开</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>晚宴之前在前院遇到了你</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>之后便去给Lee处理伤口和换药</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>戌时我出发去宴会厅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>过于简洁的证词</t>
+    <t>Dr. Ran, do you have the results?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr. Ran nodded. However, despite her usual composure, her eyes betrayed a hint of uncertainty and doubt.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the cause of the manor lord’s death?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He sustained multiple sharp-force injuries across his body.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The fatal wound was a penetrating stab through the chest and abdomen; the rest were superficial.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He died from excessive blood loss due to the severity of the wounds—it was not an instant death.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the time of death?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As is well known, temperature affects postmortem changes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tonight was windy and rainy—cold and damp.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>so rigor mortis would have set in more slowly than usual.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moreover, the deceased had been a long-time martial artist with a muscular build.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Just now, stiffness was observed beginning around the jaw, but had not yet spread to the rest of the body.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lividity had just started to appear. Based on these signs, I estimate time of death was between the beginning of the Wu hour and its midpoint.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Based on this, I can narrow down the time frame of the fight between the victim and the assailant outside the manor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The killer may have acted before the banquet, then returned and pretended as if nothing had happened.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>That coincides with the period from when the banquet was originally scheduled to start to when it actually began.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alternatively, they could have slipped away during the banquet, committed the murder, and then rejoined the event.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>According to Steward He’s testimony, the Lord was alive at the second quarter of the You hour.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This places the time of attack between the third quarter of You and the beginning of Xu—roughly a window of three quarters.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can you describe the condition of the victim’s clothing?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The clothing was completely soaked. However, due to the rain, there was little blood visible.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>His shoes and the front of his garments were caked with mud and crushed grass, especially around the knees and elbows.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>There was also a large amount of dirt under his fingernails and on his hands.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Steward He, was the lord’s clothing in this condition when you last saw him?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certainly not. As an imperial official, and with today being his birthday, the lord would have been dressed with utmost dignity.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Then it stands to reason the mud was from a struggle with the killer.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can you describe his hands in more detail?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calluses typical of martial artists were present. In addition, both palms had rope marks—</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear pressure lines running from the base of the thumb across the palm.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sir, are you suggesting the manor lord was tied up before his death?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It seems unlikely. If he had been restrained, the marks would typically be on the wrists or elbows and encircle the limb.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this case, the marks were only on the inner palms—not the backs of the hands.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The lines were clearly defined, likely inflicted shortly before death.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>That concludes today’s preliminary examination. A more thorough autopsy will be conducted tomorrow morning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>She didn’t respond, but her silence seemed like tacit consent.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When was the last time you saw the Lord?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yesterday, during a medical consultation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I was originally supposed to leave the mountain yesterday, but stayed to treat Lee’s injury.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You didn’t see the lord again at dusk today, just before the rain started?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Madam Mei suddenly took ill. The lord mentioned he wanted to ask you to treat her.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr. Ran shook her head.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Could you account for your movements before and after the banquet?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>After the banquet began, I didn’t leave the hall.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Before the banquet, I ran into you in the front yard.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Then I went to treat Lee’s wound.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>At the Xu hour, I headed to the banquet hall.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>That’s quite a concise statement.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dee-Determined</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ran-Thinking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ran-Angry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ran-Regular</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ran-Regular2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He-Angry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yao-Query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ran-Thinking2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoryScript11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -734,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEC272-F350-D34D-A243-3179172F76FB}">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -807,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -828,12 +860,12 @@
         <v>500</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="34">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -850,7 +882,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -862,18 +897,21 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:16" ht="17">
+    <row r="5" spans="1:16" ht="34">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="17">
+    <row r="6" spans="1:16" ht="34">
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
@@ -887,7 +925,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="17">
+    <row r="7" spans="1:16" ht="34">
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
@@ -908,28 +946,28 @@
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="2">
-        <v>500</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="17">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" ht="34">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -941,12 +979,15 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="34">
+    <row r="10" spans="1:16" ht="17">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -958,12 +999,15 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="17">
+    <row r="11" spans="1:16" ht="34">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -977,16 +1021,13 @@
     </row>
     <row r="12" spans="1:16" ht="34">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -994,10 +1035,13 @@
     </row>
     <row r="13" spans="1:16" ht="34">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -1009,9 +1053,15 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:16" ht="34">
+    <row r="14" spans="1:16" ht="51">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -1023,9 +1073,9 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:16" ht="34">
+    <row r="15" spans="1:16" ht="51">
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -1037,9 +1087,9 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:16" ht="34">
+    <row r="16" spans="1:16" ht="51">
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -1053,7 +1103,7 @@
     </row>
     <row r="17" spans="1:12" ht="34">
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1065,7 +1115,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="17">
+    <row r="18" spans="1:12" ht="51">
       <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1093,10 +1143,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="17">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
+    <row r="20" spans="1:12" ht="51">
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
@@ -1110,12 +1157,15 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="34">
+    <row r="21" spans="1:12" ht="17">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
@@ -1129,127 +1179,173 @@
     </row>
     <row r="22" spans="1:12" ht="34">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
       <c r="E22" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" ht="17">
+      <c r="J22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="2">
+        <v>500</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="51">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="E23" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" ht="34">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" ht="34">
       <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="51">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="17">
-      <c r="B26" s="1" t="s">
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" ht="34">
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="17">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="D27" t="s">
         <v>13</v>
       </c>
       <c r="E27" t="s">
         <v>20</v>
       </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" ht="17">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" ht="34">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="17">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" ht="34">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="17">
-      <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
+      <c r="C30" t="s">
+        <v>77</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -1257,13 +1353,19 @@
       <c r="E30" t="s">
         <v>20</v>
       </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12" ht="34">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -1271,166 +1373,365 @@
       <c r="E31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="17">
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" ht="51">
       <c r="A32" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" ht="34">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" ht="34">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D32" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="17">
-      <c r="A33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" ht="34">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="34">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" ht="34">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" ht="34">
+      <c r="B37" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D34" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="17">
-      <c r="A35" t="s">
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" ht="17">
+      <c r="A38" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D35" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="17">
-      <c r="B36" s="1" t="s">
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" ht="17">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="17">
-      <c r="A37" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" ht="34">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="17">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="34">
-      <c r="A39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="17">
-      <c r="A40" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="17">
+      <c r="C40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" ht="34">
       <c r="A41" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" ht="34">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" ht="17">
+      <c r="B43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" ht="34">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="17">
-      <c r="B42" s="1" t="s">
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" ht="17">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="17">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="C45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" ht="17">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="17">
-      <c r="A44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" ht="17">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="17">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" ht="17">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="17">
-      <c r="A46" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="C48" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" ht="17">
+      <c r="B49" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="17">
-      <c r="A47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="17">
-      <c r="B48" s="1" t="s">
-        <v>75</v>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" ht="17">
+      <c r="A50" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
7.8 History Card & Advanced Story
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/10_Ran.xlsx
+++ b/Assets/StreamingAssets/10_Ran.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7E7368-EC27-A24F-9F2F-455C8ED9F6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535D3A18-6CD7-BE4D-881A-052FBB6B54F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="85">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,10 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>What was the cause of the manor lord’s death?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>He sustained multiple sharp-force injuries across his body.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -165,10 +161,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>He died from excessive blood loss due to the severity of the wounds—it was not an instant death.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>What was the time of death?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -177,10 +169,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tonight was windy and rainy—cold and damp.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>so rigor mortis would have set in more slowly than usual.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,34 +181,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lividity had just started to appear. Based on these signs, I estimate time of death was between the beginning of the Wu hour and its midpoint.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Based on this, I can narrow down the time frame of the fight between the victim and the assailant outside the manor.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The killer may have acted before the banquet, then returned and pretended as if nothing had happened.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>That coincides with the period from when the banquet was originally scheduled to start to when it actually began.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Alternatively, they could have slipped away during the banquet, committed the murder, and then rejoined the event.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>According to Steward He’s testimony, the Lord was alive at the second quarter of the You hour.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This places the time of attack between the third quarter of You and the beginning of Xu—roughly a window of three quarters.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Can you describe the condition of the victim’s clothing?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -237,10 +197,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Steward He, was the lord’s clothing in this condition when you last saw him?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Certainly not. As an imperial official, and with today being his birthday, the lord would have been dressed with utmost dignity.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -253,26 +209,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Calluses typical of martial artists were present. In addition, both palms had rope marks—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>clear pressure lines running from the base of the thumb across the palm.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sir, are you suggesting the manor lord was tied up before his death?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>It seems unlikely. If he had been restrained, the marks would typically be on the wrists or elbows and encircle the limb.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>In this case, the marks were only on the inner palms—not the backs of the hands.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The lines were clearly defined, likely inflicted shortly before death.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -301,38 +241,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Madam Mei suddenly took ill. The lord mentioned he wanted to ask you to treat her.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dr. Ran shook her head.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Could you account for your movements before and after the banquet?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>After the banquet began, I didn’t leave the hall.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Before the banquet, I ran into you in the front yard.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Then I went to treat Lee’s wound.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>At the Xu hour, I headed to the banquet hall.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>That’s quite a concise statement.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Dee-Determined</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -370,6 +286,94 @@
   </si>
   <si>
     <t>StoryScript11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Dr. Ran shook her head.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(That’s quite a concise statement.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was the cause of the Lord’s death?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>He died from excessive blood loss due to the severity of the wounds——it was not an instant death.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tonight was windy and rainy——cold and damp.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lividity had just started to appear. Based on these signs, I estimate time of death was between the beginning of the 7 PM and 8 PM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Butler He, was the lord’s clothing in this condition when you last saw him?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calluses typical of martial artists were present. In addition, both palms had rope marks——</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clear pressure lines running from the base of the thumb across the palm.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sir, are you suggesting the Lord was tied up before his death?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this case, the marks were only on the inner palms——not the backs of the hands.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thank you so much.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Madam Mei suddenly took ill. The Lord mentioned he wanted to ask you to treat her.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Could you account for your movements before and during the banquet?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Before the banquet, I ran into you in the frontyard.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>At the 6.30 PM, I headed to the banquet hall.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(That coincides with the period from when the banquet was originally scheduled to start to when it actually began.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Based on this, I can narrow down the time frame of the fight between the victim and the assailant outside the manor.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(The killer may have acted before the banquet, then returned and pretended as if nothing had happened.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Alternatively, they could have slipped away during the banquet, committed the murder, and then rejoined the event.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(According to Butler He’s testimony, the Lord was alive at 6.30 PM.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(This places the time of attack between 6.30 PM and 8 PM—roughly a window of one and a half hour.)&lt;/color&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -768,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEC272-F350-D34D-A243-3179172F76FB}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:B56"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -860,7 +864,7 @@
         <v>500</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="34">
@@ -882,10 +886,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -902,10 +906,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -913,7 +917,7 @@
     </row>
     <row r="6" spans="1:16" ht="34">
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -927,7 +931,7 @@
     </row>
     <row r="7" spans="1:16" ht="34">
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -944,10 +948,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -964,10 +968,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -984,10 +988,10 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1004,10 +1008,10 @@
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1024,10 +1028,10 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1038,10 +1042,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -1058,10 +1062,10 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -1075,7 +1079,7 @@
     </row>
     <row r="15" spans="1:16" ht="51">
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -1089,7 +1093,7 @@
     </row>
     <row r="16" spans="1:16" ht="51">
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -1101,9 +1105,9 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="34">
+    <row r="17" spans="1:12" ht="51">
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1117,7 +1121,7 @@
     </row>
     <row r="18" spans="1:12" ht="51">
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -1131,7 +1135,7 @@
     </row>
     <row r="19" spans="1:12" ht="34">
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
@@ -1145,7 +1149,7 @@
     </row>
     <row r="20" spans="1:12" ht="51">
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
@@ -1162,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -1182,10 +1186,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -1200,7 +1204,7 @@
         <v>500</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="51">
@@ -1208,10 +1212,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -1228,10 +1232,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -1248,10 +1252,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
@@ -1268,10 +1272,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -1285,7 +1289,7 @@
     </row>
     <row r="27" spans="1:12" ht="34">
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1302,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1322,10 +1326,10 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -1342,10 +1346,10 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -1362,10 +1366,10 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -1382,10 +1386,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -1402,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -1422,10 +1426,10 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
         <v>13</v>
@@ -1442,10 +1446,10 @@
         <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -1457,12 +1461,12 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" ht="34">
+    <row r="36" spans="1:12" ht="17">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -1479,7 +1483,7 @@
     </row>
     <row r="37" spans="1:12" ht="34">
       <c r="B37" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
@@ -1496,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -1516,10 +1520,10 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -1536,10 +1540,10 @@
         <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -1556,10 +1560,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -1576,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -1593,7 +1597,7 @@
     </row>
     <row r="43" spans="1:12" ht="17">
       <c r="B43" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
         <v>13</v>
@@ -1610,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -1630,10 +1634,10 @@
         <v>24</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -1650,10 +1654,10 @@
         <v>24</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -1670,10 +1674,10 @@
         <v>24</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
         <v>13</v>
@@ -1690,10 +1694,10 @@
         <v>24</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
         <v>13</v>
@@ -1705,9 +1709,9 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" ht="17">
+    <row r="49" spans="1:12" ht="34">
       <c r="B49" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D49" t="s">
         <v>13</v>
@@ -1723,10 +1727,10 @@
     </row>
     <row r="50" spans="1:12" ht="17">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>